<commit_message>
Addition of more data sets.
</commit_message>
<xml_diff>
--- a/Data/Data_description.xlsx
+++ b/Data/Data_description.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\public\section\own_contributions\papers\2024_FA_yeast_DMI\Data\DATA_FOR_AI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\MRI_group\projects\2022_D_Xe_project\LOCAL-Git_Fanum\student_Deuterium\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB9F990-1025-4575-BD1A-3EBA24EA3043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D992242C-E9CD-472F-92C2-3C1CD748CE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_Hlk166682796" localSheetId="0">Sheet1!$J$2</definedName>
+    <definedName name="_Hlk166682796" localSheetId="0">Sheet1!$J$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,15 +37,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="109">
-  <si>
-    <t>TR[s]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="148">
   <si>
     <t>File</t>
-  </si>
-  <si>
-    <t>NS</t>
   </si>
   <si>
     <t>-</t>
@@ -86,9 +80,6 @@
     <t>Propan-2-ol-d6</t>
   </si>
   <si>
-    <t>Substrate_ppm</t>
-  </si>
-  <si>
     <t>Reaction temprature (Kelvin)</t>
   </si>
   <si>
@@ -219,42 +210,9 @@
     <t xml:space="preserve">9.031, 8.714, 8.376, 7.659 </t>
   </si>
   <si>
-    <t>Malate-d2(avg)</t>
-  </si>
-  <si>
-    <t>4.368, 2.474</t>
-  </si>
-  <si>
     <t>4.368, 2.475</t>
   </si>
   <si>
-    <t>4.368, 2.476</t>
-  </si>
-  <si>
-    <t>4.368, 2.477</t>
-  </si>
-  <si>
-    <t>4.368, 2.478</t>
-  </si>
-  <si>
-    <t>4.368, 2.479</t>
-  </si>
-  <si>
-    <t>4.368, 2.480</t>
-  </si>
-  <si>
-    <t>4.368, 2.481</t>
-  </si>
-  <si>
-    <t>4.368, 2.482</t>
-  </si>
-  <si>
-    <t>4.368, 2.483</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nicotinic acid-d4(avg) </t>
-  </si>
-  <si>
     <t>FA_20240108_2H_yeast_Nicotinamide-d4 _11.csv</t>
   </si>
   <si>
@@ -351,12 +309,6 @@
     <t>pH_after</t>
   </si>
   <si>
-    <t>Water_ppm</t>
-  </si>
-  <si>
-    <t>Substrate_N_D</t>
-  </si>
-  <si>
     <t>1, 1, 1, 1</t>
   </si>
   <si>
@@ -369,9 +321,6 @@
     <t>Expt_name</t>
   </si>
   <si>
-    <t>Substrate_mM</t>
-  </si>
-  <si>
     <t>Substrate_mM_added</t>
   </si>
   <si>
@@ -409,6 +358,174 @@
   </si>
   <si>
     <t>Metabolite_5_ppm</t>
+  </si>
+  <si>
+    <t>FA_202231122_2H_yeast_acetone-d6_1.csv</t>
+  </si>
+  <si>
+    <t>FA_202231122_2H_yeast_1_1</t>
+  </si>
+  <si>
+    <t>FA_20240206_2H_yeast_1_2</t>
+  </si>
+  <si>
+    <t>FA_20240205_2H_yeast_acetone-d6_2.csv</t>
+  </si>
+  <si>
+    <t>Substrate_N_D (no. Of deuterons)</t>
+  </si>
+  <si>
+    <t>TR[s] (Repition time)</t>
+  </si>
+  <si>
+    <t>NS (Nuber of scans or transients)</t>
+  </si>
+  <si>
+    <t>Malate-d2(sum)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicotinic acid-d4(sum) </t>
+  </si>
+  <si>
+    <t>Substrate_mM (Concentration)</t>
+  </si>
+  <si>
+    <t>Substrate_chemical shift (ppm)</t>
+  </si>
+  <si>
+    <t>Water_chemical shift (ppm)</t>
+  </si>
+  <si>
+    <t>FA_20231113_2H_yeast_pyruvate-d3_1.csv</t>
+  </si>
+  <si>
+    <t>FA_20231206_2H_yeast_pyruvate-d3_2.csv</t>
+  </si>
+  <si>
+    <t>FA_20240207_2H_yeast_pyruvate-d3_3.csv</t>
+  </si>
+  <si>
+    <t>FA_20240207_2H_yeast_pyruvate-d3_4.csv</t>
+  </si>
+  <si>
+    <t>FA_20240215_2H_yeast_pyruvate-d3_5.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pyruvate-d3 </t>
+  </si>
+  <si>
+    <t>Acetate-d3</t>
+  </si>
+  <si>
+    <t>Ethanol-d3</t>
+  </si>
+  <si>
+    <t>1.2261 </t>
+  </si>
+  <si>
+    <t>FA_20240207_2H_yeast_1_3</t>
+  </si>
+  <si>
+    <t>FA_20240215_2H_yeast_1_3</t>
+  </si>
+  <si>
+    <t>FA_20240207_2H_yeast_1_4</t>
+  </si>
+  <si>
+    <t>5..92</t>
+  </si>
+  <si>
+    <t>1g yeast in 7mL PBS (50mM)</t>
+  </si>
+  <si>
+    <t>FA_20240715_2H_yeast_1_3</t>
+  </si>
+  <si>
+    <t>FA_20240715_2H_yeast_fumarate-d2_3.csv</t>
+  </si>
+  <si>
+    <t>FA_20240715_2H_yeast_fumarate-d2_4.csv</t>
+  </si>
+  <si>
+    <t>FA_20240715_2H_yeast_1_4</t>
+  </si>
+  <si>
+    <t>FA_20240715_2H_yeast_fumarate-d2_5.csv</t>
+  </si>
+  <si>
+    <t>FA_20240715_2H_yeast_fumarate-d2_6.csv</t>
+  </si>
+  <si>
+    <t>FA_20240715_2H_yeast_1_5</t>
+  </si>
+  <si>
+    <t>FA_20240715_2H_yeast_1_6</t>
+  </si>
+  <si>
+    <t>FA_20240729_2H_yeast_fumarate-d2_6.csv</t>
+  </si>
+  <si>
+    <t>FA_20240729_2H_yeast_1_3</t>
+  </si>
+  <si>
+    <t>FA_20240729_2H_yeast_fumarate-d2_3.csv</t>
+  </si>
+  <si>
+    <t>FA_20240729_2H_yeast_fumarate-d2_8.csv</t>
+  </si>
+  <si>
+    <t>FA_20240729_2H_yeast_1_4</t>
+  </si>
+  <si>
+    <t>FA_20240729_2H_yeast_1_5</t>
+  </si>
+  <si>
+    <t>FA_20240729_2H_yeast_1_6</t>
+  </si>
+  <si>
+    <t>FA_20240729_2H_yeast_1_7</t>
+  </si>
+  <si>
+    <t>FA_20240729_2H_yeast_1_8</t>
+  </si>
+  <si>
+    <t>FA_20240729_2H_yeast_fumarate-d2_4.csv</t>
+  </si>
+  <si>
+    <t>FA_20240729_2H_yeast_fumarate-d2_5.csv</t>
+  </si>
+  <si>
+    <t>FA_20240729_2H_yeast_fumarate-d2_12.csv</t>
+  </si>
+  <si>
+    <t>FA_20240729_2H_yeast_fumarate-d2_7.csv</t>
+  </si>
+  <si>
+    <t>FA_20240729_2H_yeast_1_12</t>
+  </si>
+  <si>
+    <t>FA_20240731_2H_yeast_fumarate-d2_14.csv</t>
+  </si>
+  <si>
+    <t>FA_20240731_2H_yeast_1_14</t>
+  </si>
+  <si>
+    <t>1g yeast in 7mL PBS (320mM)</t>
+  </si>
+  <si>
+    <t>PBS (320mM)</t>
+  </si>
+  <si>
+    <t>1g yeast in 7mL PBS (200mM)</t>
+  </si>
+  <si>
+    <t>PBS (200mM)</t>
+  </si>
+  <si>
+    <t>1g yeast in 7mL PBS (25mM)</t>
+  </si>
+  <si>
+    <t>PBS (25mM)</t>
   </si>
 </sst>
 </file>
@@ -759,10 +876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA25"/>
+  <dimension ref="A1:AA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +888,7 @@
     <col min="3" max="3" width="40.85546875" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" customWidth="1"/>
     <col min="7" max="9" width="34.7109375" customWidth="1"/>
-    <col min="10" max="10" width="23.85546875" customWidth="1"/>
+    <col min="10" max="10" width="34.28515625" customWidth="1"/>
     <col min="11" max="12" width="34.7109375" customWidth="1"/>
     <col min="13" max="13" width="29.7109375" customWidth="1"/>
     <col min="14" max="14" width="25.7109375" customWidth="1"/>
@@ -790,85 +907,85 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="X1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z1" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="X1" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>107</v>
-      </c>
       <c r="AA1" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -876,10 +993,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="D2" s="2">
         <v>17.5</v>
@@ -892,7 +1009,7 @@
         <v>140</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H2" s="2">
         <v>6</v>
@@ -905,25 +1022,25 @@
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2">
-        <v>5.0599999999999996</v>
+        <v>5.2</v>
       </c>
       <c r="M2" s="1">
         <v>310</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q2" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
@@ -932,70 +1049,67 @@
       <c r="W2" s="1">
         <v>1.2010000000000001</v>
       </c>
-      <c r="AA2" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="D3" s="2">
-        <v>11.5</v>
+        <v>17.5</v>
       </c>
       <c r="E3" s="2">
         <v>8</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F5" si="0">E3*D3</f>
-        <v>92</v>
+        <f>E3*D3</f>
+        <v>140</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>92</v>
+        <v>3</v>
+      </c>
+      <c r="H3" s="2">
+        <v>6</v>
       </c>
       <c r="I3" s="2">
         <v>15</v>
       </c>
       <c r="J3" s="1">
-        <v>6.6529999999999996</v>
+        <v>2.323</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2">
-        <v>5.6</v>
+        <v>5.31</v>
       </c>
       <c r="M3" s="1">
         <v>310</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q3" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
-      <c r="W3" s="1" t="s">
-        <v>46</v>
+      <c r="W3" s="1">
+        <v>1.2010000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
@@ -1003,61 +1117,64 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2">
-        <v>11.5</v>
+        <v>17.5</v>
       </c>
       <c r="E4" s="2">
         <v>8</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="0"/>
-        <v>92</v>
+        <f>E4*D4</f>
+        <v>140</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>92</v>
+        <v>3</v>
+      </c>
+      <c r="H4" s="2">
+        <v>6</v>
       </c>
       <c r="I4" s="2">
         <v>15</v>
       </c>
       <c r="J4" s="1">
-        <v>6.6529999999999996</v>
+        <v>2.323</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2">
-        <v>5.63</v>
+        <v>5.0599999999999996</v>
       </c>
       <c r="M4" s="1">
         <v>310</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q4" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
-      <c r="W4" s="1" t="s">
-        <v>47</v>
+      <c r="W4" s="1">
+        <v>1.2010000000000001</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
@@ -1065,10 +1182,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2">
         <v>11.5</v>
@@ -1077,14 +1194,14 @@
         <v>8</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F5:F6" si="0">E5*D5</f>
         <v>92</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="I5" s="2">
         <v>15</v>
@@ -1100,26 +1217,26 @@
         <v>310</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q5" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
       <c r="W5" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
@@ -1127,26 +1244,26 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2">
-        <v>2.5</v>
+        <v>11.5</v>
       </c>
       <c r="E6" s="2">
         <v>8</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" ref="F6:F19" si="1">E6*D6</f>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>92</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="I6" s="2">
         <v>15</v>
@@ -1156,32 +1273,32 @@
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2">
-        <v>5.89</v>
+        <v>5.63</v>
       </c>
       <c r="M6" s="1">
         <v>310</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q6" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
@@ -1189,26 +1306,26 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2">
-        <v>11.5</v>
+        <v>2.5</v>
       </c>
       <c r="E7" s="2">
         <v>8</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="1"/>
-        <v>92</v>
+        <f t="shared" ref="F7:F20" si="1">E7*D7</f>
+        <v>20</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="I7" s="2">
         <v>15</v>
@@ -1218,32 +1335,32 @@
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2">
-        <v>6</v>
+        <v>5.89</v>
       </c>
       <c r="M7" s="1">
         <v>310</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q7" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
@@ -1251,10 +1368,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2">
         <v>11.5</v>
@@ -1267,10 +1384,10 @@
         <v>92</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="I8" s="2">
         <v>15</v>
@@ -1280,32 +1397,32 @@
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2">
-        <v>7.08</v>
+        <v>6</v>
       </c>
       <c r="M8" s="1">
         <v>310</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>28</v>
+        <v>117</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q8" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
       <c r="W8" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
@@ -1313,10 +1430,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D9" s="2">
         <v>11.5</v>
@@ -1329,10 +1446,10 @@
         <v>92</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="I9" s="2">
         <v>15</v>
@@ -1342,32 +1459,32 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2">
-        <v>5.69</v>
+        <v>7.08</v>
       </c>
       <c r="M9" s="1">
         <v>310</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q9" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
@@ -1375,26 +1492,26 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2">
-        <v>2.5</v>
+        <v>11.5</v>
       </c>
       <c r="E10" s="2">
         <v>8</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="I10" s="2">
         <v>15</v>
@@ -1404,32 +1521,32 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2">
-        <v>5.67</v>
+        <v>5.69</v>
       </c>
       <c r="M10" s="1">
         <v>310</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q10" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
       <c r="W10" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -1437,10 +1554,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2">
         <v>2.5</v>
@@ -1453,10 +1570,10 @@
         <v>20</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="I11" s="2">
         <v>15</v>
@@ -1466,32 +1583,32 @@
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2">
-        <v>5.97</v>
+        <v>5.67</v>
       </c>
       <c r="M11" s="1">
         <v>310</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q11" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
       <c r="W11" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
@@ -1499,10 +1616,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2">
         <v>2.5</v>
@@ -1515,10 +1632,10 @@
         <v>20</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="I12" s="2">
         <v>15</v>
@@ -1528,32 +1645,32 @@
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2">
-        <v>7.11</v>
+        <v>5.97</v>
       </c>
       <c r="M12" s="1">
         <v>310</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>29</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q12" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
       <c r="W12" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
@@ -1561,63 +1678,61 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D13" s="2">
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
       <c r="E13" s="2">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="1"/>
-        <v>168</v>
+        <v>20</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="I13" s="2">
-        <v>5</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K13" s="2">
-        <v>5.63</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="J13" s="1">
+        <v>6.6529999999999996</v>
+      </c>
+      <c r="K13" s="2"/>
       <c r="L13" s="2">
-        <v>5.93</v>
+        <v>7.11</v>
       </c>
       <c r="M13" s="1">
         <v>310</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="Q13" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
@@ -1625,63 +1740,63 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="D14" s="2">
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
       <c r="E14" s="2">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="1"/>
-        <v>168</v>
+        <v>20</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="I14" s="2">
-        <v>5</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
+      </c>
+      <c r="J14" s="1">
+        <v>6.6529999999999996</v>
       </c>
       <c r="K14" s="2">
-        <v>5.52</v>
+        <v>7.29</v>
       </c>
       <c r="L14" s="2">
-        <v>6.13</v>
+        <v>6.96</v>
       </c>
       <c r="M14" s="1">
         <v>310</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>97</v>
+        <v>26</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="Q14" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
@@ -1689,63 +1804,63 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="D15" s="2">
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
       <c r="E15" s="2">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="1"/>
-        <v>168</v>
+        <v>20</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="I15" s="2">
-        <v>5</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
+      </c>
+      <c r="J15" s="1">
+        <v>6.6529999999999996</v>
       </c>
       <c r="K15" s="2">
-        <v>5.48</v>
+        <v>7.18</v>
       </c>
       <c r="L15" s="2">
-        <v>5.98</v>
+        <v>7.03</v>
       </c>
       <c r="M15" s="1">
         <v>310</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>97</v>
+        <v>143</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="Q15" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
@@ -1753,63 +1868,63 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="D16" s="2">
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
       <c r="E16" s="2">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="1"/>
-        <v>168</v>
+        <v>20</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="I16" s="2">
-        <v>5</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
+      </c>
+      <c r="J16" s="1">
+        <v>6.6529999999999996</v>
       </c>
       <c r="K16" s="2">
-        <v>5.61</v>
+        <v>6.92</v>
       </c>
       <c r="L16" s="2">
-        <v>5.92</v>
+        <v>6.87</v>
       </c>
       <c r="M16" s="1">
         <v>310</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>21</v>
+        <v>144</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="Q16" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
       <c r="W16" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
@@ -1817,63 +1932,63 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="D17" s="2">
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
       <c r="E17" s="2">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="1"/>
-        <v>168</v>
+        <v>20</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="I17" s="2">
-        <v>5</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
+      </c>
+      <c r="J17" s="1">
+        <v>6.6529999999999996</v>
       </c>
       <c r="K17" s="2">
-        <v>6.9</v>
+        <v>5.98</v>
       </c>
       <c r="L17" s="2">
-        <v>6.48</v>
+        <v>5.86</v>
       </c>
       <c r="M17" s="1">
         <v>310</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>66</v>
+        <v>146</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>97</v>
+        <v>147</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="Q17" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
       <c r="W17" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
@@ -1881,63 +1996,62 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>68</v>
+        <v>125</v>
       </c>
       <c r="D18" s="2">
-        <v>2.1</v>
+        <v>11.5</v>
       </c>
       <c r="E18" s="2">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="1"/>
-        <v>168</v>
+        <v>92</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="I18" s="2">
-        <v>5</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
+      </c>
+      <c r="J18" s="1">
+        <v>6.6529999999999996</v>
       </c>
       <c r="K18" s="2">
-        <v>6.8</v>
+        <v>7.01</v>
       </c>
       <c r="L18" s="2">
-        <v>6.29</v>
+        <v>6.98</v>
       </c>
       <c r="M18" s="1">
         <v>310</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>66</v>
+        <v>142</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>97</v>
+        <v>143</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="Q18" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
@@ -1945,63 +2059,62 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>70</v>
+        <v>128</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>71</v>
+        <v>127</v>
       </c>
       <c r="D19" s="2">
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
       <c r="E19" s="2">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" si="1"/>
-        <v>168</v>
+        <v>20</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="I19" s="2">
-        <v>5</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
+      </c>
+      <c r="J19" s="1">
+        <v>6.6529999999999996</v>
       </c>
       <c r="K19" s="2">
-        <v>6.81</v>
+        <v>7.31</v>
       </c>
       <c r="L19" s="2">
-        <v>6.13</v>
+        <v>7.24</v>
       </c>
       <c r="M19" s="1">
         <v>310</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>97</v>
+        <v>26</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="Q19" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
       <c r="W19" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
@@ -2009,63 +2122,62 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="D20" s="2">
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
       <c r="E20" s="2">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" ref="F20:F23" si="2">E20*D20</f>
-        <v>168</v>
+        <v>20</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>75</v>
+        <v>7</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="I20" s="2">
-        <v>5</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
+      </c>
+      <c r="J20" s="1">
+        <v>6.6529999999999996</v>
       </c>
       <c r="K20" s="2">
-        <v>6.7</v>
+        <v>5.93</v>
       </c>
       <c r="L20" s="2">
-        <v>6.04</v>
+        <v>5.82</v>
       </c>
       <c r="M20" s="1">
         <v>310</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>66</v>
+        <v>146</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>97</v>
+        <v>147</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="Q20" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
       <c r="W20" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
@@ -2073,63 +2185,62 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="E21" s="2">
+        <v>8</v>
+      </c>
+      <c r="F21" s="2">
+        <v>20</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="2">
-        <v>2.1</v>
-      </c>
-      <c r="E21" s="2">
-        <v>80</v>
-      </c>
-      <c r="F21" s="2">
-        <f t="shared" si="2"/>
-        <v>168</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="I21" s="2">
-        <v>5</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
+      </c>
+      <c r="J21" s="1">
+        <v>6.6529999999999996</v>
       </c>
       <c r="K21" s="2">
-        <v>6.57</v>
+        <v>6.97</v>
       </c>
       <c r="L21" s="2">
-        <v>5.95</v>
+        <v>6.91</v>
       </c>
       <c r="M21" s="1">
         <v>310</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>66</v>
+        <v>142</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>97</v>
+        <v>143</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="Q21" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
@@ -2137,63 +2248,62 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="D22" s="2">
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
       <c r="E22" s="2">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="F22" s="2">
-        <f t="shared" si="2"/>
-        <v>168</v>
+        <v>20</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="I22" s="2">
-        <v>5</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
+      </c>
+      <c r="J22" s="1">
+        <v>6.6529999999999996</v>
       </c>
       <c r="K22" s="2">
-        <v>6.3</v>
+        <v>6.83</v>
       </c>
       <c r="L22" s="2">
-        <v>5.91</v>
+        <v>6.75</v>
       </c>
       <c r="M22" s="1">
         <v>310</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>66</v>
+        <v>144</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="Q22" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
       <c r="W22" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
@@ -2201,112 +2311,1414 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>82</v>
+        <v>126</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="D23" s="2">
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
       <c r="E23" s="2">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" si="2"/>
-        <v>168</v>
+        <v>20</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="I23" s="2">
-        <v>5</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
+      </c>
+      <c r="J23" s="1">
+        <v>6.6529999999999996</v>
       </c>
       <c r="K23" s="2">
-        <v>5.83</v>
+        <v>6.42</v>
       </c>
       <c r="L23" s="2">
-        <v>5.89</v>
+        <v>6.37</v>
       </c>
       <c r="M23" s="1">
         <v>310</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="Q23" s="2">
-        <v>7.4</v>
+        <v>4.7</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
       <c r="W23" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D24" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="F24" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" s="2">
+        <v>15</v>
+      </c>
+      <c r="J24" s="1">
+        <v>6.6529999999999996</v>
+      </c>
+      <c r="K24" s="2">
+        <v>5.84</v>
+      </c>
+      <c r="L24" s="2">
+        <v>3.92</v>
+      </c>
+      <c r="M24" s="1">
+        <v>310</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
+      <c r="W24" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I25" s="2">
+        <v>15</v>
+      </c>
+      <c r="J25" s="1">
+        <v>6.6529999999999996</v>
+      </c>
+      <c r="K25" s="2">
+        <v>6.38</v>
+      </c>
+      <c r="L25" s="2">
+        <v>5.81</v>
+      </c>
+      <c r="M25" s="1">
+        <v>310</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
+      <c r="W25" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D26" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="F26" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I26" s="2">
+        <v>15</v>
+      </c>
+      <c r="J26" s="1">
+        <v>6.6529999999999996</v>
+      </c>
+      <c r="K26" s="2">
+        <v>5.43</v>
+      </c>
+      <c r="L26" s="2">
+        <v>5.76</v>
+      </c>
+      <c r="M26" s="1">
+        <v>310</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="E27" s="2">
+        <v>80</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" ref="F27:F42" si="2">E27*D27</f>
+        <v>168</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I27" s="2">
+        <v>5</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K27" s="2">
+        <v>5.63</v>
+      </c>
+      <c r="L27" s="2">
+        <v>5.93</v>
+      </c>
+      <c r="M27" s="1">
+        <v>310</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="E28" s="2">
+        <v>80</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I28" s="2">
+        <v>5</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K28" s="2">
+        <v>5.52</v>
+      </c>
+      <c r="L28" s="2">
+        <v>6.13</v>
+      </c>
+      <c r="M28" s="1">
+        <v>310</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="E29" s="2">
+        <v>80</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I29" s="2">
+        <v>5</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K29" s="2">
+        <v>5.48</v>
+      </c>
+      <c r="L29" s="2">
+        <v>5.98</v>
+      </c>
+      <c r="M29" s="1">
+        <v>310</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="E30" s="2">
+        <v>80</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I30" s="2">
+        <v>5</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" s="2">
+        <v>5.61</v>
+      </c>
+      <c r="L30" s="2">
+        <v>5.92</v>
+      </c>
+      <c r="M30" s="1">
+        <v>310</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R30" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="E31" s="2">
+        <v>80</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I31" s="2">
+        <v>5</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K31" s="2">
+        <v>6.9</v>
+      </c>
+      <c r="L31" s="2">
+        <v>6.48</v>
+      </c>
+      <c r="M31" s="1">
+        <v>310</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="E32" s="2">
+        <v>80</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I32" s="2">
+        <v>5</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K32" s="2">
+        <v>6.8</v>
+      </c>
+      <c r="L32" s="2">
+        <v>6.29</v>
+      </c>
+      <c r="M32" s="1">
+        <v>310</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="E33" s="2">
+        <v>80</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I33" s="2">
+        <v>5</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K33" s="2">
+        <v>6.81</v>
+      </c>
+      <c r="L33" s="2">
+        <v>6.13</v>
+      </c>
+      <c r="M33" s="1">
+        <v>310</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O33" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="E34" s="2">
+        <v>80</v>
+      </c>
+      <c r="F34" s="2">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I34" s="2">
+        <v>5</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" s="2">
+        <v>6.7</v>
+      </c>
+      <c r="L34" s="2">
+        <v>6.04</v>
+      </c>
+      <c r="M34" s="1">
+        <v>310</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q34" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="E35" s="2">
+        <v>80</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I35" s="2">
+        <v>5</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K35" s="2">
+        <v>6.57</v>
+      </c>
+      <c r="L35" s="2">
+        <v>5.95</v>
+      </c>
+      <c r="M35" s="1">
+        <v>310</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R35" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="E36" s="2">
+        <v>80</v>
+      </c>
+      <c r="F36" s="2">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I36" s="2">
+        <v>5</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K36" s="2">
+        <v>6.3</v>
+      </c>
+      <c r="L36" s="2">
+        <v>5.91</v>
+      </c>
+      <c r="M36" s="1">
+        <v>310</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q36" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R36" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="E37" s="2">
+        <v>80</v>
+      </c>
+      <c r="F37" s="2">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I37" s="2">
+        <v>5</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K37" s="2">
+        <v>5.83</v>
+      </c>
+      <c r="L37" s="2">
+        <v>5.89</v>
+      </c>
+      <c r="M37" s="1">
+        <v>310</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q37" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="E38" s="2">
+        <v>8</v>
+      </c>
+      <c r="F38" s="2">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I38" s="2">
+        <v>15</v>
+      </c>
+      <c r="J38" s="2">
+        <v>2.468</v>
+      </c>
+      <c r="K38" s="2">
+        <v>6.11</v>
+      </c>
+      <c r="L38" s="2">
+        <v>5.7</v>
+      </c>
+      <c r="M38" s="2">
+        <v>310</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q38" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R38" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="S38" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="X38">
+        <v>1.9775</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="E39" s="2">
+        <v>8</v>
+      </c>
+      <c r="F39" s="2">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I39" s="2">
+        <v>15</v>
+      </c>
+      <c r="J39" s="2">
+        <v>2.468</v>
+      </c>
+      <c r="K39" s="2">
+        <v>5.94</v>
+      </c>
+      <c r="L39" s="2">
+        <v>5.53</v>
+      </c>
+      <c r="M39" s="2">
+        <v>310</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q39" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R39" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="S39" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="W39" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="X39">
+        <v>1.9775</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>106</v>
+      </c>
+      <c r="C40" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="E40" s="2">
+        <v>8</v>
+      </c>
+      <c r="F40" s="2">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I40" s="2">
+        <v>15</v>
+      </c>
+      <c r="J40" s="2">
+        <v>2.468</v>
+      </c>
+      <c r="K40" t="s">
+        <v>116</v>
+      </c>
+      <c r="L40" s="2">
+        <v>5.67</v>
+      </c>
+      <c r="M40" s="2">
+        <v>310</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R40" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="S40" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="W40" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="X40">
+        <v>1.9775</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D41" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="E41" s="2">
+        <v>8</v>
+      </c>
+      <c r="F41" s="2">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" s="2">
+        <v>15</v>
+      </c>
+      <c r="J41" s="2">
+        <v>2.468</v>
+      </c>
+      <c r="K41" s="2">
+        <v>6.03</v>
+      </c>
+      <c r="L41" s="2">
+        <v>5.61</v>
+      </c>
+      <c r="M41" s="2">
+        <v>310</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q41" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R41" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="S41" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="W41" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="X41">
+        <v>1.9775</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="E42" s="2">
+        <v>8</v>
+      </c>
+      <c r="F42" s="2">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I42" s="2">
+        <v>15</v>
+      </c>
+      <c r="J42" s="2">
+        <v>2.468</v>
+      </c>
+      <c r="K42" s="2">
+        <v>5.95</v>
+      </c>
+      <c r="L42" s="2">
+        <v>5.58</v>
+      </c>
+      <c r="M42" s="2">
+        <v>310</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R42" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="S42" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="W42" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="X42">
+        <v>1.9775</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
+      <c r="S46" s="2"/>
+      <c r="T46" s="2"/>
+      <c r="U46" s="2"/>
+      <c r="V46" s="2"/>
+      <c r="W46" s="1"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+      <c r="U47" s="2"/>
+      <c r="V47" s="2"/>
+      <c r="W47" s="2"/>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+      <c r="S48" s="2"/>
+      <c r="W48" s="2"/>
+    </row>
+    <row r="49" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2"/>
+      <c r="W49" s="2"/>
+    </row>
+    <row r="50" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2"/>
+      <c r="W50" s="2"/>
+    </row>
+    <row r="51" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2"/>
+      <c r="S51" s="2"/>
+      <c r="W51" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
try out peak finder via sum and derivate --> in progress correct typos filenames in data description
</commit_message>
<xml_diff>
--- a/Data/Data_description.xlsx
+++ b/Data/Data_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\MRI_group\projects\2022_D_Xe_project\LOCAL-Git_Fanum\student_Deuterium\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive\Data_Science\Sem2_Application_Project\MoinCC-AI4metabolomics\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D992242C-E9CD-472F-92C2-3C1CD748CE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C61B42B-50B2-45B4-9699-555C667A902F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -360,9 +360,6 @@
     <t>Metabolite_5_ppm</t>
   </si>
   <si>
-    <t>FA_202231122_2H_yeast_acetone-d6_1.csv</t>
-  </si>
-  <si>
     <t>FA_202231122_2H_yeast_1_1</t>
   </si>
   <si>
@@ -526,6 +523,9 @@
   </si>
   <si>
     <t>PBS (25mM)</t>
+  </si>
+  <si>
+    <t>FA_20231122_2H_yeast_acetone-d6_1.csv</t>
   </si>
 </sst>
 </file>
@@ -598,7 +598,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -879,33 +879,33 @@
   <dimension ref="A1:AA51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="45" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" customWidth="1"/>
-    <col min="7" max="9" width="34.7109375" customWidth="1"/>
-    <col min="10" max="10" width="34.28515625" customWidth="1"/>
-    <col min="11" max="12" width="34.7109375" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" customWidth="1"/>
-    <col min="14" max="14" width="25.7109375" customWidth="1"/>
-    <col min="15" max="15" width="21.28515625" customWidth="1"/>
-    <col min="16" max="17" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="40.81640625" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" customWidth="1"/>
+    <col min="7" max="9" width="34.7265625" customWidth="1"/>
+    <col min="10" max="10" width="34.26953125" customWidth="1"/>
+    <col min="11" max="12" width="34.7265625" customWidth="1"/>
+    <col min="13" max="13" width="29.7265625" customWidth="1"/>
+    <col min="14" max="14" width="25.7265625" customWidth="1"/>
+    <col min="15" max="15" width="21.26953125" customWidth="1"/>
+    <col min="16" max="17" width="23.81640625" customWidth="1"/>
     <col min="18" max="18" width="20" customWidth="1"/>
-    <col min="19" max="19" width="17.5703125" customWidth="1"/>
-    <col min="20" max="20" width="18.7109375" customWidth="1"/>
-    <col min="21" max="21" width="17.7109375" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" customWidth="1"/>
-    <col min="23" max="23" width="24.7109375" customWidth="1"/>
-    <col min="24" max="24" width="18.7109375" customWidth="1"/>
-    <col min="27" max="27" width="15.42578125" customWidth="1"/>
+    <col min="19" max="19" width="17.54296875" customWidth="1"/>
+    <col min="20" max="20" width="18.7265625" customWidth="1"/>
+    <col min="21" max="21" width="17.7265625" customWidth="1"/>
+    <col min="22" max="22" width="16.7265625" customWidth="1"/>
+    <col min="23" max="23" width="24.7265625" customWidth="1"/>
+    <col min="24" max="24" width="18.7265625" customWidth="1"/>
+    <col min="27" max="27" width="15.453125" customWidth="1"/>
     <col min="28" max="28" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -916,10 +916,10 @@
         <v>78</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>17</v>
@@ -928,13 +928,13 @@
         <v>77</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>73</v>
@@ -955,7 +955,7 @@
         <v>79</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>81</v>
@@ -988,15 +988,15 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="D2" s="2">
         <v>17.5</v>
@@ -1050,15 +1050,15 @@
         <v>1.2010000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="2">
         <v>17.5</v>
@@ -1112,7 +1112,7 @@
         <v>1.2010000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>4.7</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
@@ -1239,7 +1239,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>4.7</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
@@ -1301,7 +1301,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" ref="F7:F20" si="1">E7*D7</f>
+        <f t="shared" ref="F7:F17" si="1">E7*D7</f>
         <v>20</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -1353,7 +1353,7 @@
         <v>4.7</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
@@ -1363,7 +1363,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>310</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>80</v>
@@ -1415,7 +1415,7 @@
         <v>4.7</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
@@ -1425,7 +1425,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>4.7</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
@@ -1487,7 +1487,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>4.7</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
@@ -1549,7 +1549,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>4.7</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
@@ -1611,7 +1611,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>4.7</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
@@ -1673,7 +1673,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>4.7</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
@@ -1735,7 +1735,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>4.7</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
@@ -1799,15 +1799,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D15" s="2">
         <v>2.5</v>
@@ -1841,10 +1841,10 @@
         <v>310</v>
       </c>
       <c r="N15" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O15" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="P15" s="2" t="s">
         <v>4</v>
@@ -1853,7 +1853,7 @@
         <v>4.7</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
@@ -1863,15 +1863,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="D16" s="2">
         <v>2.5</v>
@@ -1905,10 +1905,10 @@
         <v>310</v>
       </c>
       <c r="N16" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="O16" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="P16" s="2" t="s">
         <v>4</v>
@@ -1917,7 +1917,7 @@
         <v>4.7</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
@@ -1927,15 +1927,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D17" s="2">
         <v>2.5</v>
@@ -1969,10 +1969,10 @@
         <v>310</v>
       </c>
       <c r="N17" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="O17" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>4</v>
@@ -1981,7 +1981,7 @@
         <v>4.7</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
@@ -1991,15 +1991,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D18" s="2">
         <v>11.5</v>
@@ -2032,10 +2032,10 @@
         <v>310</v>
       </c>
       <c r="N18" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O18" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>4</v>
@@ -2044,7 +2044,7 @@
         <v>4.7</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
@@ -2054,15 +2054,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D19" s="2">
         <v>2.5</v>
@@ -2107,7 +2107,7 @@
         <v>4.7</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
@@ -2117,15 +2117,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D20" s="2">
         <v>2.5</v>
@@ -2158,10 +2158,10 @@
         <v>310</v>
       </c>
       <c r="N20" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="O20" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="P20" s="2" t="s">
         <v>4</v>
@@ -2170,7 +2170,7 @@
         <v>4.7</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
@@ -2180,15 +2180,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D21" s="2">
         <v>2.5</v>
@@ -2221,10 +2221,10 @@
         <v>310</v>
       </c>
       <c r="N21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O21" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="P21" s="2" t="s">
         <v>4</v>
@@ -2233,7 +2233,7 @@
         <v>4.7</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
@@ -2243,15 +2243,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D22" s="2">
         <v>2.5</v>
@@ -2284,10 +2284,10 @@
         <v>310</v>
       </c>
       <c r="N22" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="O22" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="P22" s="2" t="s">
         <v>4</v>
@@ -2296,7 +2296,7 @@
         <v>4.7</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
@@ -2306,15 +2306,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D23" s="2">
         <v>2.5</v>
@@ -2359,7 +2359,7 @@
         <v>4.7</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
@@ -2369,15 +2369,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D24" s="2">
         <v>2.5</v>
@@ -2422,7 +2422,7 @@
         <v>4.7</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
@@ -2432,15 +2432,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D25" s="2">
         <v>2.5</v>
@@ -2473,7 +2473,7 @@
         <v>310</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O25" s="2" t="s">
         <v>80</v>
@@ -2485,7 +2485,7 @@
         <v>4.7</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
@@ -2495,15 +2495,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="D26" s="2">
         <v>2.5</v>
@@ -2536,10 +2536,10 @@
         <v>310</v>
       </c>
       <c r="N26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O26" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="P26" s="2" t="s">
         <v>4</v>
@@ -2548,7 +2548,7 @@
         <v>4.7</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
@@ -2558,7 +2558,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>4.7</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
@@ -2622,7 +2622,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>4.7</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
@@ -2686,7 +2686,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>4.7</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
@@ -2750,7 +2750,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>4.7</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
@@ -2814,7 +2814,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>4.7</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
@@ -2878,7 +2878,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>4.7</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
@@ -2942,7 +2942,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>4.7</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
@@ -3006,7 +3006,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>4.7</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
@@ -3070,7 +3070,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>4.7</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S35" s="2"/>
       <c r="T35" s="2"/>
@@ -3134,7 +3134,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>4.7</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S36" s="2"/>
       <c r="T36" s="2"/>
@@ -3198,7 +3198,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>4.7</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S37" s="2"/>
       <c r="T37" s="2"/>
@@ -3262,15 +3262,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D38" s="2">
         <v>15.5</v>
@@ -3283,7 +3283,7 @@
         <v>124</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>76</v>
@@ -3316,30 +3316,30 @@
         <v>4.7</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
       <c r="W38" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="X38">
         <v>1.9775</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D39" s="2">
         <v>15.5</v>
@@ -3352,7 +3352,7 @@
         <v>124</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>76</v>
@@ -3385,27 +3385,27 @@
         <v>4.7</v>
       </c>
       <c r="R39" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="S39" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="W39" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="S39" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="W39" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="X39">
         <v>1.9775</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D40" s="2">
         <v>15.5</v>
@@ -3418,7 +3418,7 @@
         <v>124</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>76</v>
@@ -3430,7 +3430,7 @@
         <v>2.468</v>
       </c>
       <c r="K40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L40" s="2">
         <v>5.67</v>
@@ -3451,27 +3451,27 @@
         <v>4.7</v>
       </c>
       <c r="R40" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="S40" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="W40" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="S40" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="W40" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="X40">
         <v>1.9775</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D41" s="2">
         <v>15.5</v>
@@ -3484,7 +3484,7 @@
         <v>124</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>76</v>
@@ -3517,27 +3517,27 @@
         <v>4.7</v>
       </c>
       <c r="R41" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="S41" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="W41" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="S41" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="W41" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="X41">
         <v>1.9775</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D42" s="2">
         <v>15.5</v>
@@ -3550,7 +3550,7 @@
         <v>124</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>76</v>
@@ -3583,19 +3583,19 @@
         <v>4.7</v>
       </c>
       <c r="R42" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="S42" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="W42" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="S42" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="W42" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="X42">
         <v>1.9775</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -3619,7 +3619,7 @@
       <c r="V46" s="2"/>
       <c r="W46" s="1"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -3643,7 +3643,7 @@
       <c r="V47" s="2"/>
       <c r="W47" s="2"/>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -3664,7 +3664,7 @@
       <c r="S48" s="2"/>
       <c r="W48" s="2"/>
     </row>
-    <row r="49" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
@@ -3682,7 +3682,7 @@
       <c r="S49" s="2"/>
       <c r="W49" s="2"/>
     </row>
-    <row r="50" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
@@ -3701,7 +3701,7 @@
       <c r="S50" s="2"/>
       <c r="W50" s="2"/>
     </row>
-    <row r="51" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:23" x14ac:dyDescent="0.35">
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>

</xml_diff>